<commit_message>
updated license (as Agrovoc) from CC BY-NC-SA to CC BY
</commit_message>
<xml_diff>
--- a/LandVoc-concepts.xlsx
+++ b/LandVoc-concepts.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LandVoc concepts" sheetId="1" r:id="rId1"/>
     <sheet name="What is LandVoc" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -4036,6 +4036,9 @@
       </rPr>
       <t>, published d.d. February 24th 2018.</t>
     </r>
+  </si>
+  <si>
+    <t>continuum in land rights</t>
   </si>
   <si>
     <r>
@@ -4105,11 +4108,8 @@
       </rPr>
       <t xml:space="preserve"> through browsing and searching.
 This file contains all concepts currently in LandVoc and the translations into four languages (English, French, Spanish and Portuguese). This file does not contain synonyms or relationships between different concepts.
-LandVoc content in English, French, Spanish and Portuguese is licensed under Creative Commons Attribution-NonCommercial-ShareAlike 3.0 IGO License (CC BY-NC-SA 3.0 IGO).</t>
+LandVoc content in English, French, Spanish and Portuguese is licensed under Creative Commons Attribution 3.0 IGO License (CC BY 3.0 IGO).</t>
     </r>
-  </si>
-  <si>
-    <t>continuum in land rights</t>
   </si>
 </sst>
 </file>
@@ -4678,7 +4678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
@@ -5434,7 +5434,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>574</v>
@@ -14701,7 +14701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:G4"/>
     </sheetView>
   </sheetViews>
@@ -14725,7 +14725,7 @@
     </row>
     <row r="3" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>

</xml_diff>